<commit_message>
add my name  - add my email - add my repo link
</commit_message>
<xml_diff>
--- a/Open Source task.xlsx
+++ b/Open Source task.xlsx
@@ -1,42 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
-  <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\legion\Desktop\open-source\Security-Task\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\mmm\Security-Task\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{655120EA-671F-4435-B8F2-FC3A0DB523E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1A782380-5C03-4ABF-949C-B3350E41F3A7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <si>
     <t>name</t>
   </si>
@@ -47,20 +29,29 @@
     <t>Repo Link</t>
   </si>
   <si>
+    <t>السيد اسامه رجب السيد</t>
+  </si>
+  <si>
+    <t>heikalsayed@gmail.com</t>
+  </si>
+  <si>
     <t>https://github.com/0xkillua/Security-Task.git</t>
   </si>
   <si>
-    <t>heikalsayed@gmail.com</t>
-  </si>
-  <si>
-    <t>السيد اسامه رجب السيد</t>
+    <t xml:space="preserve">محمد شريف محمد احمد </t>
+  </si>
+  <si>
+    <t>mohammedsherifhegazy10@gmail.com</t>
+  </si>
+  <si>
+    <t>https://github.com/sherry100000/Security-Task</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -73,7 +64,6 @@
       <sz val="11"/>
       <color theme="10"/>
       <name val="Aptos Narrow"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -86,19 +76,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.89999084444715716"/>
+        <fgColor theme="3" tint="0.899990844447157"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
   <borders count="2">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
+    <border/>
     <border>
       <left style="thin">
         <color indexed="64"/>
@@ -112,7 +96,6 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="2">
@@ -125,19 +108,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -146,10 +121,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="0E2841"/>
@@ -318,6 +293,7 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
+          <a:tileRect/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -344,24 +320,25 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
+          <a:tileRect/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="12700" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="19050" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="25400" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -422,56 +399,29 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
+          <a:tileRect/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults>
-    <a:lnDef>
-      <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </a:style>
-    </a:lnDef>
-  </a:objectDefaults>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88B88C28-23A0-4FB2-A45B-5BE272931FEB}">
-  <dimension ref="A1:C2"/>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" rightToLeft="1" workbookViewId="0" topLeftCell="C1">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="46.44140625" customWidth="1"/>
-    <col min="2" max="2" width="49.6640625" customWidth="1"/>
-    <col min="3" max="3" width="51.6640625" customWidth="1"/>
+    <col min="1" max="1" width="46.44141" customWidth="1"/>
+    <col min="2" max="2" width="49.66406" customWidth="1"/>
+    <col min="3" max="3" width="51.66406" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -482,22 +432,32 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>3</v>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{A364EA89-B4FA-4322-9DA7-87C8CDF404AF}"/>
-    <hyperlink ref="B2" r:id="rId2" xr:uid="{65319477-3938-45F9-8CEB-9746D877D7C0}"/>
+    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>